<commit_message>
swapped excl and quest
</commit_message>
<xml_diff>
--- a/Keymap.xlsx
+++ b/Keymap.xlsx
@@ -249,58 +249,58 @@
     <t>€</t>
   </si>
   <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>leestekens</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>+-</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>capslock</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>{</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>leestekens</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>+-</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>(</t>
-  </si>
-  <si>
-    <t>)</t>
-  </si>
-  <si>
-    <t>capslock</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>!</t>
   </si>
   <si>
     <t>;</t>
@@ -510,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -525,15 +525,14 @@
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="1"/>
     <xf fontId="0" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2030,7 +2029,7 @@
       <c r="L25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="M25" s="12" t="s">
         <v>78</v>
       </c>
       <c r="N25" s="2" t="s">
@@ -2102,13 +2101,13 @@
       <c r="J26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="13" t="s">
         <v>85</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="14" t="s">
         <v>87</v>
       </c>
       <c r="N26" s="6" t="s">
@@ -2182,7 +2181,7 @@
       <c r="L27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="12" t="s">
         <v>95</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -2446,16 +2445,16 @@
       <c r="J32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="15" t="s">
         <v>30</v>
       </c>
       <c r="O32" s="2" t="s">
@@ -2478,7 +2477,7 @@
       <c r="X32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Y32" s="14"/>
+      <c r="Y32" s="15"/>
       <c r="Z32" s="2"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
@@ -2540,11 +2539,11 @@
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="2"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15" t="s">
+      <c r="V33" s="16"/>
+      <c r="W33" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="X33" s="15"/>
+      <c r="X33" s="16"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AB33" s="1"/>
@@ -2707,16 +2706,16 @@
       <c r="J37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="M37" s="16" t="s">
+      <c r="M37" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="N37" s="16" t="s">
+      <c r="N37" s="17" t="s">
         <v>108</v>
       </c>
       <c r="O37" s="2" t="s">
@@ -2727,15 +2726,15 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="17" t="s">
+      <c r="U37" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16" t="s">
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="Y37" s="16"/>
+      <c r="Y37" s="17"/>
       <c r="Z37" s="2"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
@@ -2785,7 +2784,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="20" t="s">
+      <c r="U38" s="18" t="s">
         <v>113</v>
       </c>
       <c r="V38" s="4"/>
@@ -2829,29 +2828,29 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="17"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7" t="s">
         <v>3</v>
       </c>
       <c r="R39" s="1"/>
-      <c r="S39" s="21"/>
+      <c r="S39" s="20"/>
       <c r="T39" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U39" s="17" t="s">
+      <c r="U39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="15" t="s">
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="Y39" s="15"/>
+      <c r="Y39" s="16"/>
       <c r="Z39" s="2"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
@@ -2890,13 +2889,13 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="22" t="s">
+      <c r="N40" s="21" t="s">
         <v>6</v>
       </c>
       <c r="O40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P40" s="23" t="s">
+      <c r="P40" s="22" t="s">
         <v>38</v>
       </c>
       <c r="Q40" s="7" t="s">

</xml_diff>